<commit_message>
wetland sampling oct15 &16
</commit_message>
<xml_diff>
--- a/Wetlands/SamplingNotes/SamplingData_Wetland-06_2022-10-15.xlsx
+++ b/Wetlands/SamplingNotes/SamplingData_Wetland-06_2022-10-15.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kriddie/Documents/Ecuador2022/Wetlands/SamplingNotes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A23F3DA8-8BBE-3444-B154-A8D78D2B6E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA04115C-F435-3844-8644-D9AB7D8B448A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11220" yWindow="2900" windowWidth="27640" windowHeight="16940" xr2:uid="{849C4510-753D-8A4A-96BF-125E2BFDB151}"/>
+    <workbookView xWindow="720" yWindow="4320" windowWidth="27640" windowHeight="16940" xr2:uid="{849C4510-753D-8A4A-96BF-125E2BFDB151}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -440,7 +440,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,7 +521,7 @@
         <v>2</v>
       </c>
       <c r="C10">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D10" s="3">
         <v>0.48958333333333331</v>

</xml_diff>